<commit_message>
HERE WE GO AGAIN
</commit_message>
<xml_diff>
--- a/Martin/ANM/EksamenE2022/Formler.xlsx
+++ b/Martin/ANM/EksamenE2022/Formler.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\45201\Documents\Uni\Git2\Martin\ANM\EksamenE2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CA65DD-BB23-491E-9859-FED4BB48A62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073E16AB-5B16-4E60-941B-7673359BE1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1527339-D591-4740-B24E-3FD46250A267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B1527339-D591-4740-B24E-3FD46250A267}"/>
   </bookViews>
   <sheets>
     <sheet name="Bisection" sheetId="1" r:id="rId1"/>
+    <sheet name="New-Raphson" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,6 +40,36 @@
     <author>Martin Teit Andersen</author>
   </authors>
   <commentList>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{7565925E-FAAE-4D2A-945B-0FB6B97D5D83}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin Teit Andersen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Halløj! 
+Når i vil anvende denne tabel, så skal i kun ændre input i de gulefelter.
+Kigger vi på iteration 1, når funktionerne:
+- f_1
+- f_ur
+- f_xr
+har fået angivet sin funktion, så skal du huske at klikke på den nederste markerede firkant, der kaster cellen til mængden af iterationer.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K8" authorId="0" shapeId="0" xr:uid="{D922DF10-BDE8-4D19-BE58-CD05A8991AB2}">
       <text>
         <r>
@@ -91,8 +122,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Martin Teit Andersen</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{1B8A8DED-9A63-4E6C-B847-A5A510BA0DC2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Martin Teit Andersen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skal differentieres i enten MatLab, MathCad eller lign.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Iteration</t>
   </si>
@@ -142,15 +207,49 @@
     <t>f_xu</t>
   </si>
   <si>
-    <t>Check if eta_a &lt; e_s</t>
+    <t>LÆS MIG!</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Check if eta_a =&lt; e_s</t>
+  </si>
+  <si>
+    <t>Newton-Raphsons metode</t>
+  </si>
+  <si>
+    <t>Funktion:</t>
+  </si>
+  <si>
+    <t>f(x) = x^2-4</t>
+  </si>
+  <si>
+    <t>Differentieret:</t>
+  </si>
+  <si>
+    <t>f'(x) = 2x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>f(x)</t>
+  </si>
+  <si>
+    <t>f'(x)</t>
+  </si>
+  <si>
+    <t>Iterationer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -181,7 +280,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +335,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -265,9 +370,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -276,8 +382,17 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E3F470-CC0C-4331-93E6-50AE060F4B6A}">
   <dimension ref="B2:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,12 +728,15 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>50</v>
       </c>
     </row>
@@ -626,7 +744,7 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>200</v>
       </c>
     </row>
@@ -634,713 +752,912 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10">
-        <v>0.05</v>
+      <c r="C6" s="14">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="L8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <f>C4</f>
         <v>50</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="9">
         <f>C5</f>
         <v>200</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="10">
         <f>(C9+D9)/2</f>
         <v>125</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <f>SIN(10*C9)+COS(3*C9)</f>
         <v>0.23147900115589898</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="5">
         <f>SIN(10*D9)+COS(3*D9)</f>
         <v>-6.8983974416768734E-2</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="5">
         <f>SIN(10*E9)+COS(3*E9)</f>
         <v>-0.75459089348005293</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="6">
         <f>F9*H9</f>
         <v>-0.17467194630410002</v>
       </c>
-      <c r="J9" s="6" t="str">
+      <c r="J9" s="13" t="str">
         <f>IF(I9&gt;0,"TRUE","FALSE")</f>
         <v>FALSE</v>
       </c>
+      <c r="K9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>2</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <f>IF(J9="TRUE",E9,C9)</f>
         <v>50</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <f>IF(J9="FALSE",E9,D9)</f>
         <v>125</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="10">
         <f>(C10+D10)/2</f>
         <v>87.5</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <f t="shared" ref="F10:F23" si="0">SIN(10*C10)+COS(3*C10)</f>
         <v>0.23147900115589898</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="5">
         <f t="shared" ref="G10:G23" si="1">SIN(10*D10)+COS(3*D10)</f>
         <v>-0.75459089348005293</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="5">
         <f t="shared" ref="H10:H23" si="2">SIN(10*E10)+COS(3*E10)</f>
         <v>1.1738837348957101</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="6">
         <f>F10*H10</f>
         <v>0.27172943442681508</v>
       </c>
-      <c r="J10" s="6" t="str">
+      <c r="J10" s="13" t="str">
         <f t="shared" ref="J10:J23" si="3">IF(I10&gt;0,"TRUE","FALSE")</f>
         <v>TRUE</v>
       </c>
       <c r="K10" s="11">
-        <f>ABS((E10-E9)/E10)*100</f>
-        <v>42.857142857142854</v>
-      </c>
-      <c r="L10" t="str">
-        <f>IF(K10&lt;$C$6,"TRUE","FALSE")</f>
+        <f>ABS((E10-E9)/E10)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="L10" s="12" t="str">
+        <f>IF(K10&lt;=$C$6,"TRUE","FALSE")</f>
         <v>FALSE</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>3</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <f t="shared" ref="C11:C23" si="4">IF(J10="TRUE",E10,C10)</f>
         <v>87.5</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="9">
         <f t="shared" ref="D11:D23" si="5">IF(J10="FALSE",E10,D10)</f>
         <v>125</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="10">
         <f>(C11+D11)/2</f>
         <v>106.25</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>1.1738837348957101</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
         <v>-0.75459089348005293</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="5">
         <f t="shared" si="2"/>
         <v>0.47719010639489445</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="6">
         <f>F11*H11</f>
         <v>0.56016570435011992</v>
       </c>
-      <c r="J11" s="6" t="str">
+      <c r="J11" s="13" t="str">
         <f t="shared" si="3"/>
         <v>TRUE</v>
       </c>
       <c r="K11" s="11">
-        <f t="shared" ref="K11:K23" si="6">ABS((E11-E10)/E11)*100</f>
-        <v>17.647058823529413</v>
-      </c>
-      <c r="L11" t="str">
-        <f>IF(K11&lt;$C$6,"TRUE","FALSE")</f>
+        <f t="shared" ref="K11:K23" si="6">ABS((E11-E10)/E11)</f>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="L11" s="12" t="str">
+        <f t="shared" ref="L11:L23" si="7">IF(K11&lt;=$C$6,"TRUE","FALSE")</f>
         <v>FALSE</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>4</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="8">
         <f t="shared" si="4"/>
         <v>106.25</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="9">
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="10">
         <f>(C12+D12)/2</f>
         <v>115.625</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="5">
         <f t="shared" si="0"/>
         <v>0.47719010639489445</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="5">
         <f t="shared" si="1"/>
         <v>-0.75459089348005293</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="5">
         <f t="shared" si="2"/>
         <v>0.41109105459128881</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="6">
         <f>F12*H12</f>
         <v>0.19616858407840648</v>
       </c>
-      <c r="J12" s="6" t="str">
+      <c r="J12" s="13" t="str">
         <f t="shared" si="3"/>
         <v>TRUE</v>
       </c>
       <c r="K12" s="11">
         <f t="shared" si="6"/>
-        <v>8.1081081081081088</v>
-      </c>
-      <c r="L12" t="str">
-        <f>IF(K12&lt;$C$6,"TRUE","FALSE")</f>
+        <v>8.1081081081081086E-2</v>
+      </c>
+      <c r="L12" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>FALSE</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>5</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="8">
         <f t="shared" si="4"/>
         <v>115.625</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="9">
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="10">
         <f>(C13+D13)/2</f>
         <v>120.3125</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="5">
         <f t="shared" si="0"/>
         <v>0.41109105459128881</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="5">
         <f t="shared" si="1"/>
         <v>-0.75459089348005293</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="5">
         <f t="shared" si="2"/>
         <v>-0.83606010773396044</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="6">
         <f>F13*H13</f>
         <v>-0.34369683139006035</v>
       </c>
-      <c r="J13" s="6" t="str">
+      <c r="J13" s="13" t="str">
         <f t="shared" si="3"/>
         <v>FALSE</v>
       </c>
       <c r="K13" s="11">
         <f t="shared" si="6"/>
-        <v>3.8961038961038961</v>
-      </c>
-      <c r="L13" t="str">
-        <f>IF(K13&lt;$C$6,"TRUE","FALSE")</f>
+        <v>3.896103896103896E-2</v>
+      </c>
+      <c r="L13" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>FALSE</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>6</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="8">
         <f t="shared" si="4"/>
         <v>115.625</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="9">
         <f t="shared" si="5"/>
         <v>120.3125</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="10">
         <f>(C14+D14)/2</f>
         <v>117.96875</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="5">
         <f t="shared" si="0"/>
         <v>0.41109105459128881</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="5">
         <f t="shared" si="1"/>
         <v>-0.83606010773396044</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="5">
         <f t="shared" si="2"/>
         <v>-1.4589947384340258</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="6">
         <f>F14*H14</f>
         <v>-0.59977968566598527</v>
       </c>
-      <c r="J14" s="6" t="str">
+      <c r="J14" s="13" t="str">
         <f t="shared" si="3"/>
         <v>FALSE</v>
       </c>
       <c r="K14" s="11">
         <f t="shared" si="6"/>
-        <v>1.9867549668874174</v>
-      </c>
-      <c r="L14" t="str">
-        <f>IF(K14&lt;$C$6,"TRUE","FALSE")</f>
+        <v>1.9867549668874173E-2</v>
+      </c>
+      <c r="L14" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>FALSE</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
+      <c r="B15" s="4">
         <v>7</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="8">
         <f t="shared" si="4"/>
         <v>115.625</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <f t="shared" si="5"/>
         <v>117.96875</v>
       </c>
-      <c r="E15" s="9">
-        <f t="shared" ref="E15:E23" si="7">(C15+D15)/2</f>
+      <c r="E15" s="10">
+        <f t="shared" ref="E15:E23" si="8">(C15+D15)/2</f>
         <v>116.796875</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="5">
         <f t="shared" si="0"/>
         <v>0.41109105459128881</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
         <v>-1.4589947384340258</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="5">
         <f t="shared" si="2"/>
         <v>-0.54419438585897317</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="6">
         <f>F15*H15</f>
         <v>-0.22371344398542403</v>
       </c>
-      <c r="J15" s="6" t="str">
+      <c r="J15" s="13" t="str">
         <f t="shared" si="3"/>
         <v>FALSE</v>
       </c>
       <c r="K15" s="11">
         <f t="shared" si="6"/>
-        <v>1.0033444816053512</v>
-      </c>
-      <c r="L15" t="str">
-        <f>IF(K15&lt;$C$6,"TRUE","FALSE")</f>
+        <v>1.0033444816053512E-2</v>
+      </c>
+      <c r="L15" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>FALSE</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <v>8</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="8">
         <f t="shared" si="4"/>
         <v>115.625</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="9">
         <f t="shared" si="5"/>
         <v>116.796875</v>
       </c>
-      <c r="E16" s="9">
-        <f t="shared" si="7"/>
+      <c r="E16" s="10">
+        <f t="shared" si="8"/>
         <v>116.2109375</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="5">
         <f t="shared" si="0"/>
         <v>0.41109105459128881</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="5">
         <f t="shared" si="1"/>
         <v>-0.54419438585897317</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="5">
         <f t="shared" si="2"/>
         <v>-1.2727425228776785</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="6">
         <f>F16*H16</f>
         <v>-0.52321306595296235</v>
       </c>
-      <c r="J16" s="6" t="str">
+      <c r="J16" s="13" t="str">
         <f t="shared" si="3"/>
         <v>FALSE</v>
       </c>
       <c r="K16" s="11">
         <f t="shared" si="6"/>
-        <v>0.50420168067226889</v>
-      </c>
-      <c r="L16" t="str">
-        <f>IF(K16&lt;$C$6,"TRUE","FALSE")</f>
+        <v>5.0420168067226894E-3</v>
+      </c>
+      <c r="L16" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>FALSE</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>9</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="8">
         <f t="shared" si="4"/>
         <v>115.625</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="9">
         <f t="shared" si="5"/>
         <v>116.2109375</v>
       </c>
-      <c r="E17" s="9">
-        <f t="shared" si="7"/>
+      <c r="E17" s="10">
+        <f t="shared" si="8"/>
         <v>115.91796875</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="5">
         <f t="shared" si="0"/>
         <v>0.41109105459128881</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="5">
         <f t="shared" si="1"/>
         <v>-1.2727425228776785</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="5">
         <f t="shared" si="2"/>
         <v>-0.50321045825728994</v>
       </c>
-      <c r="I17" s="5">
-        <f t="shared" ref="I17:I23" si="8">F17*H17</f>
+      <c r="I17" s="6">
+        <f t="shared" ref="I17:I23" si="9">F17*H17</f>
         <v>-0.20686531796635504</v>
       </c>
-      <c r="J17" s="6" t="str">
+      <c r="J17" s="13" t="str">
         <f t="shared" si="3"/>
         <v>FALSE</v>
       </c>
       <c r="K17" s="11">
         <f t="shared" si="6"/>
-        <v>0.25273799494524007</v>
-      </c>
-      <c r="L17" t="str">
-        <f>IF(K17&lt;$C$6,"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>2.527379949452401E-3</v>
+      </c>
+      <c r="L17" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>TRUE</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="3">
+      <c r="B18" s="4">
         <v>10</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="8">
         <f t="shared" si="4"/>
         <v>115.625</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="9">
         <f t="shared" si="5"/>
         <v>115.91796875</v>
       </c>
-      <c r="E18" s="9">
-        <f t="shared" si="7"/>
+      <c r="E18" s="10">
+        <f t="shared" si="8"/>
         <v>115.771484375</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="5">
         <f t="shared" si="0"/>
         <v>0.41109105459128881</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="5">
         <f t="shared" si="1"/>
         <v>-0.50321045825728994</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="5">
         <f t="shared" si="2"/>
         <v>0.83161076851644145</v>
       </c>
-      <c r="I18" s="5">
-        <f t="shared" si="8"/>
+      <c r="I18" s="6">
+        <f t="shared" si="9"/>
         <v>0.34186774783889606</v>
       </c>
-      <c r="J18" s="6" t="str">
+      <c r="J18" s="13" t="str">
         <f t="shared" si="3"/>
         <v>TRUE</v>
       </c>
       <c r="K18" s="11">
         <f t="shared" si="6"/>
-        <v>0.12652889076339097</v>
-      </c>
-      <c r="L18" t="str">
-        <f>IF(K18&lt;$C$6,"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>1.2652889076339097E-3</v>
+      </c>
+      <c r="L18" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>TRUE</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
+      <c r="B19" s="4">
         <v>11</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="8">
         <f t="shared" si="4"/>
         <v>115.771484375</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="9">
         <f t="shared" si="5"/>
         <v>115.91796875</v>
       </c>
-      <c r="E19" s="9">
-        <f t="shared" si="7"/>
+      <c r="E19" s="10">
+        <f t="shared" si="8"/>
         <v>115.8447265625</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="5">
         <f t="shared" si="0"/>
         <v>0.83161076851644145</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="5">
         <f t="shared" si="1"/>
         <v>-0.50321045825728994</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="5">
         <f t="shared" si="2"/>
         <v>0.33913605178249151</v>
       </c>
-      <c r="I19" s="5">
-        <f t="shared" si="8"/>
+      <c r="I19" s="6">
+        <f t="shared" si="9"/>
         <v>0.28202919265446946</v>
       </c>
-      <c r="J19" s="6" t="str">
+      <c r="J19" s="13" t="str">
         <f t="shared" si="3"/>
         <v>TRUE</v>
       </c>
       <c r="K19" s="11">
         <f t="shared" si="6"/>
-        <v>6.3224446786090613E-2</v>
-      </c>
-      <c r="L19" t="str">
-        <f>IF(K19&lt;$C$6,"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>6.3224446786090617E-4</v>
+      </c>
+      <c r="L19" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v>TRUE</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <v>12</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="8">
         <f t="shared" si="4"/>
         <v>115.8447265625</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="9">
         <f t="shared" si="5"/>
         <v>115.91796875</v>
       </c>
-      <c r="E20" s="9">
-        <f t="shared" si="7"/>
+      <c r="E20" s="10">
+        <f t="shared" si="8"/>
         <v>115.88134765625</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="5">
         <f t="shared" si="0"/>
         <v>0.33913605178249151</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="5">
         <f t="shared" si="1"/>
         <v>-0.50321045825728994</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="5">
         <f t="shared" si="2"/>
         <v>-5.7021300223018989E-2</v>
       </c>
-      <c r="I20" s="5">
-        <f t="shared" si="8"/>
+      <c r="I20" s="6">
+        <f t="shared" si="9"/>
         <v>-1.9337978625138762E-2</v>
       </c>
-      <c r="J20" s="6" t="str">
+      <c r="J20" s="13" t="str">
         <f t="shared" si="3"/>
         <v>FALSE</v>
       </c>
       <c r="K20" s="11">
         <f t="shared" si="6"/>
-        <v>3.1602233224481198E-2</v>
-      </c>
-      <c r="L20" t="str">
-        <f>IF(K20&lt;$C$6,"TRUE","FALSE")</f>
+        <v>3.1602233224481196E-4</v>
+      </c>
+      <c r="L20" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>TRUE</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>13</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="8">
         <f t="shared" si="4"/>
         <v>115.8447265625</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="9">
         <f t="shared" si="5"/>
         <v>115.88134765625</v>
       </c>
-      <c r="E21" s="9">
-        <f t="shared" si="7"/>
+      <c r="E21" s="10">
+        <f t="shared" si="8"/>
         <v>115.863037109375</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="5">
         <f t="shared" si="0"/>
         <v>0.33913605178249151</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="5">
         <f t="shared" si="1"/>
         <v>-5.7021300223018989E-2</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="5">
         <f t="shared" si="2"/>
         <v>0.1500872983920134</v>
       </c>
-      <c r="I21" s="5">
-        <f t="shared" si="8"/>
+      <c r="I21" s="6">
+        <f t="shared" si="9"/>
         <v>5.0900013799368114E-2</v>
       </c>
-      <c r="J21" s="6" t="str">
+      <c r="J21" s="13" t="str">
         <f t="shared" si="3"/>
         <v>TRUE</v>
       </c>
       <c r="K21" s="11">
         <f t="shared" si="6"/>
-        <v>1.5803613759679716E-2</v>
-      </c>
-      <c r="L21" t="str">
-        <f>IF(K21&lt;$C$6,"TRUE","FALSE")</f>
+        <v>1.5803613759679715E-4</v>
+      </c>
+      <c r="L21" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>TRUE</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>14</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="8">
         <f t="shared" si="4"/>
         <v>115.863037109375</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="9">
         <f t="shared" si="5"/>
         <v>115.88134765625</v>
       </c>
-      <c r="E22" s="9">
-        <f t="shared" si="7"/>
+      <c r="E22" s="10">
+        <f t="shared" si="8"/>
         <v>115.8721923828125</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="5">
         <f t="shared" si="0"/>
         <v>0.1500872983920134</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="5">
         <f t="shared" si="1"/>
         <v>-5.7021300223018989E-2</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="5">
         <f t="shared" si="2"/>
         <v>4.846385523426433E-2</v>
       </c>
-      <c r="I22" s="5">
-        <f t="shared" si="8"/>
+      <c r="I22" s="6">
+        <f t="shared" si="9"/>
         <v>7.2738091017723709E-3</v>
       </c>
-      <c r="J22" s="6" t="str">
+      <c r="J22" s="13" t="str">
         <f t="shared" si="3"/>
         <v>TRUE</v>
       </c>
       <c r="K22" s="11">
         <f t="shared" si="6"/>
-        <v>7.9011825436540329E-3</v>
-      </c>
-      <c r="L22" t="str">
-        <f>IF(K22&lt;$C$6,"TRUE","FALSE")</f>
+        <v>7.9011825436540333E-5</v>
+      </c>
+      <c r="L22" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>TRUE</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>15</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="8">
         <f t="shared" si="4"/>
         <v>115.8721923828125</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="9">
         <f t="shared" si="5"/>
         <v>115.88134765625</v>
       </c>
-      <c r="E23" s="9">
-        <f t="shared" si="7"/>
+      <c r="E23" s="10">
+        <f t="shared" si="8"/>
         <v>115.87677001953125</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="5">
         <f t="shared" si="0"/>
         <v>4.846385523426433E-2</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="5">
         <f t="shared" si="1"/>
         <v>-5.7021300223018989E-2</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="5">
         <f t="shared" si="2"/>
         <v>-3.8388981746716455E-3</v>
       </c>
-      <c r="I23" s="5">
-        <f t="shared" si="8"/>
+      <c r="I23" s="6">
+        <f t="shared" si="9"/>
         <v>-1.860478053963682E-4</v>
       </c>
-      <c r="J23" s="6" t="str">
+      <c r="J23" s="13" t="str">
         <f t="shared" si="3"/>
         <v>FALSE</v>
       </c>
       <c r="K23" s="11">
         <f t="shared" si="6"/>
-        <v>3.950435206278558E-3</v>
-      </c>
-      <c r="L23" t="str">
-        <f>IF(K23&lt;$C$6,"TRUE","FALSE")</f>
+        <v>3.9504352062785581E-5</v>
+      </c>
+      <c r="L23" s="12" t="str">
+        <f t="shared" si="7"/>
         <v>TRUE</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F87973F-A0A5-4B50-9A97-CAF83418955F}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <f>C5</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="5">
+        <f>C8^2-4</f>
+        <v>21</v>
+      </c>
+      <c r="E8" s="5">
+        <f>2*C8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <f>B8+1</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="8">
+        <f>$C8-$D8/$E8</f>
+        <v>2.9</v>
+      </c>
+      <c r="D9" s="10">
+        <f>$C9^2-4</f>
+        <v>4.41</v>
+      </c>
+      <c r="E9" s="7">
+        <f>2*$C9</f>
+        <v>5.8</v>
+      </c>
+      <c r="F9" s="17">
+        <f>ABS(($C9-$C8)/$C9)</f>
+        <v>0.72413793103448276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <f t="shared" ref="B10:B13" si="0">B9+1</f>
+        <v>2</v>
+      </c>
+      <c r="C10" s="8">
+        <f>$C9-$D9/$E9</f>
+        <v>2.1396551724137929</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" ref="D10:D13" si="1">$C10^2-4</f>
+        <v>0.57812425683709812</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" ref="E10:E13" si="2">2*$C10</f>
+        <v>4.2793103448275858</v>
+      </c>
+      <c r="F10" s="17">
+        <f t="shared" ref="F10:F13" si="3">ABS(($C10-$C9)/$C10)</f>
+        <v>0.35535858178888002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" ref="C10:C13" si="4">$C10-$D10/$E10</f>
+        <v>2.0045576426130207</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="1"/>
+        <v>1.8251342558270878E-2</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="2"/>
+        <v>4.0091152852260414</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="3"/>
+        <v>6.7395183320678745E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C12" s="8">
+        <f t="shared" si="4"/>
+        <v>2.0000051812194735</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="1"/>
+        <v>2.0724904739033434E-5</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="2"/>
+        <v>4.0000103624389469</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="3"/>
+        <v>2.2762247999634994E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C13" s="8">
+        <f t="shared" si="4"/>
+        <v>2.0000000000067111</v>
+      </c>
+      <c r="D13" s="10">
+        <f t="shared" si="1"/>
+        <v>2.6844304557016585E-11</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="2"/>
+        <v>4.0000000000134222</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" si="3"/>
+        <v>2.590606381183325E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>